<commit_message>
Readme mit Beispiel ergänzt
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -65,30 +65,30 @@
     <t>Klimaneutralität C</t>
   </si>
   <si>
+    <t>Mia</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>Emma</t>
+  </si>
+  <si>
     <t>Hannah</t>
   </si>
   <si>
-    <t>Mia</t>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Anna</t>
+  </si>
+  <si>
+    <t>Sophie</t>
   </si>
   <si>
     <t>Emilia</t>
   </si>
   <si>
-    <t>Emma</t>
-  </si>
-  <si>
-    <t>Marie</t>
-  </si>
-  <si>
-    <t>Anna</t>
-  </si>
-  <si>
-    <t>Sophie</t>
-  </si>
-  <si>
-    <t>Sophia</t>
-  </si>
-  <si>
     <t>Lina</t>
   </si>
   <si>
@@ -101,18 +101,21 @@
     <t>Lilly</t>
   </si>
   <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Lea</t>
+  </si>
+  <si>
+    <t>Noah</t>
+  </si>
+  <si>
+    <t>Johanna</t>
+  </si>
+  <si>
     <t>Lena</t>
   </si>
   <si>
-    <t>Emily</t>
-  </si>
-  <si>
-    <t>Lea</t>
-  </si>
-  <si>
-    <t>Noah</t>
-  </si>
-  <si>
     <t>Luisa</t>
   </si>
   <si>
@@ -125,21 +128,18 @@
     <t>Henry</t>
   </si>
   <si>
+    <t>Laura</t>
+  </si>
+  <si>
     <t>Leonie</t>
   </si>
   <si>
-    <t>Johanna</t>
-  </si>
-  <si>
     <t>Leon</t>
   </si>
   <si>
     <t>Finn</t>
   </si>
   <si>
-    <t>Laura</t>
-  </si>
-  <si>
     <t>Emil</t>
   </si>
   <si>
@@ -170,42 +170,42 @@
     <t>Julian</t>
   </si>
   <si>
+    <t>Jakob</t>
+  </si>
+  <si>
+    <t>Jonathan</t>
+  </si>
+  <si>
+    <t>Raphael</t>
+  </si>
+  <si>
+    <t>Ida</t>
+  </si>
+  <si>
+    <t>Felix</t>
+  </si>
+  <si>
     <t>Paul</t>
   </si>
   <si>
-    <t>Jakob</t>
-  </si>
-  <si>
-    <t>Jonathan</t>
-  </si>
-  <si>
-    <t>Raphael</t>
-  </si>
-  <si>
-    <t>Ida</t>
-  </si>
-  <si>
-    <t>Felix</t>
-  </si>
-  <si>
     <t>Max</t>
   </si>
   <si>
     <t>Moritz</t>
   </si>
   <si>
+    <t>Niklas</t>
+  </si>
+  <si>
     <t>Mathilda</t>
   </si>
   <si>
-    <t>Niklas</t>
+    <t>Pia</t>
   </si>
   <si>
     <t>Ella</t>
   </si>
   <si>
-    <t>Pia</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -221,7 +221,7 @@
     <t>Parameter</t>
   </si>
   <si>
-    <t>Seed für Zufallszahlen: "01/22/2022, 16:30:25"</t>
+    <t>Seed für Zufallszahlen: "01/22/2022, 16:54:24"</t>
   </si>
   <si>
     <t>Eingabe-Datei: input.xlsx</t>
@@ -715,52 +715,52 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" t="s">
-        <v>44</v>
-      </c>
-      <c r="M2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" t="s">
-        <v>50</v>
-      </c>
-      <c r="O2" t="s">
-        <v>41</v>
-      </c>
       <c r="P2" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="Q2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="R2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="S2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="T2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="U2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="V2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -786,43 +786,43 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" t="s">
         <v>29</v>
       </c>
-      <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
       <c r="N3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="O3" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="P3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Q3" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="R3" t="s">
         <v>49</v>
       </c>
       <c r="S3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T3" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:22">
@@ -842,43 +842,43 @@
         <v>0.5384615384615384</v>
       </c>
       <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
       <c r="J4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="K4" t="s">
         <v>28</v>
       </c>
       <c r="L4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O4" t="s">
         <v>35</v>
       </c>
-      <c r="N4" t="s">
-        <v>36</v>
-      </c>
-      <c r="O4" t="s">
-        <v>33</v>
-      </c>
       <c r="P4" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="Q4" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="R4" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="S4" t="s">
         <v>47</v>
@@ -904,43 +904,43 @@
         <v>17</v>
       </c>
       <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="H5" t="s">
-        <v>27</v>
-      </c>
       <c r="I5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
         <v>21</v>
       </c>
-      <c r="J5" t="s">
-        <v>36</v>
-      </c>
       <c r="K5" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="L5" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="O5" t="s">
         <v>55</v>
       </c>
       <c r="P5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>54</v>
+      </c>
+      <c r="R5" t="s">
         <v>56</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>40</v>
-      </c>
-      <c r="R5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -960,22 +960,22 @@
         <v>0.7777777777777778</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G6" t="s">
         <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L6" t="s">
         <v>45</v>
@@ -993,13 +993,13 @@
         <v>57</v>
       </c>
       <c r="Q6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="R6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="S6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -1019,22 +1019,22 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
         <v>20</v>
       </c>
       <c r="H7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
         <v>28</v>
       </c>
-      <c r="I7" t="s">
-        <v>29</v>
-      </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L7" t="s">
         <v>46</v>
@@ -1043,7 +1043,7 @@
         <v>49</v>
       </c>
       <c r="N7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1072,19 +1072,19 @@
         <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="M8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N8" t="s">
         <v>43</v>
@@ -1093,7 +1093,7 @@
         <v>47</v>
       </c>
       <c r="P8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:22">
@@ -1122,10 +1122,10 @@
         <v>24</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K9" t="s">
         <v>41</v>
@@ -1134,7 +1134,7 @@
         <v>47</v>
       </c>
       <c r="M9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1154,19 +1154,19 @@
         <v>0.8</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
         <v>42</v>
@@ -1175,7 +1175,7 @@
         <v>48</v>
       </c>
       <c r="M10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:22">
@@ -1201,10 +1201,10 @@
         <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J11" t="s">
         <v>40</v>
@@ -1216,7 +1216,7 @@
         <v>49</v>
       </c>
       <c r="M11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1269,13 +1269,13 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1304,7 +1304,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1316,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1444,7 +1444,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1482,10 +1482,10 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1587,7 +1587,7 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1599,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1619,7 +1619,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1654,13 +1654,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1689,10 +1689,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1774,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -1794,7 +1794,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -1803,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -1864,7 +1864,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -1873,7 +1873,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1902,7 +1902,7 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1914,7 +1914,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1943,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1969,7 +1969,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -2007,10 +2007,10 @@
         <v>44</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -2039,13 +2039,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>0</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -2054,7 +2054,7 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -2077,7 +2077,7 @@
         <v>45</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -2086,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2109,7 +2109,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>0</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2179,10 +2179,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -2252,7 +2252,7 @@
         <v>46</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -2319,10 +2319,10 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -2360,10 +2360,10 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -2389,7 +2389,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -2398,7 +2398,7 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2427,10 +2427,10 @@
         <v>56</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -2462,10 +2462,10 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -2503,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -2564,7 +2564,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -2602,10 +2602,10 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -2643,10 +2643,10 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2704,19 +2704,19 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43">
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -2809,7 +2809,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -2844,10 +2844,10 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2879,13 +2879,13 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -2967,13 +2967,13 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -3014,7 +3014,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -3072,13 +3072,13 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -3142,7 +3142,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -3180,10 +3180,10 @@
         <v>23</v>
       </c>
       <c r="B8">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3247,7 +3247,7 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -3285,7 +3285,7 @@
         <v>25</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -3297,7 +3297,7 @@
         <v>-1</v>
       </c>
       <c r="F11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -3317,7 +3317,7 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -3326,7 +3326,7 @@
         <v>-1</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -3352,13 +3352,13 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>-1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -3387,10 +3387,10 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C14">
         <v>-1</v>
@@ -3472,7 +3472,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>-1</v>
@@ -3501,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -3527,7 +3527,7 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3562,7 +3562,7 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -3571,7 +3571,7 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -3600,7 +3600,7 @@
         <v>26</v>
       </c>
       <c r="B20">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -3612,7 +3612,7 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>-1</v>
@@ -3641,7 +3641,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>-1</v>
@@ -3705,10 +3705,10 @@
         <v>44</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C23">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -3737,13 +3737,13 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>-1</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -3752,7 +3752,7 @@
         <v>-1</v>
       </c>
       <c r="F24">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -3775,7 +3775,7 @@
         <v>45</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -3784,7 +3784,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -3807,7 +3807,7 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>-1</v>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>-1</v>
@@ -3877,10 +3877,10 @@
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -3950,7 +3950,7 @@
         <v>46</v>
       </c>
       <c r="B30">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -4017,10 +4017,10 @@
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -4058,10 +4058,10 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -4087,7 +4087,7 @@
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -4096,7 +4096,7 @@
         <v>-1</v>
       </c>
       <c r="D34">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E34">
         <v>-1</v>
@@ -4125,10 +4125,10 @@
         <v>56</v>
       </c>
       <c r="B35">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D35">
         <v>-1</v>
@@ -4160,10 +4160,10 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C36">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -4201,7 +4201,7 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E37">
         <v>-1</v>
@@ -4227,7 +4227,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4262,7 +4262,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -4300,10 +4300,10 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C40">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -4341,10 +4341,10 @@
         <v>1</v>
       </c>
       <c r="D41">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -4402,19 +4402,19 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43">
         <v>-1</v>
       </c>
       <c r="C43">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D43">
         <v>-1</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -4437,7 +4437,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -4472,7 +4472,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45">
         <v>-1</v>
@@ -4507,7 +4507,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -4542,10 +4542,10 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -4577,13 +4577,13 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -4650,7 +4650,7 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>4</v>
@@ -4664,21 +4664,21 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -4692,7 +4692,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -4720,7 +4720,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -4762,7 +4762,7 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -4790,44 +4790,44 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12">
         <v>3</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13">
         <v>6</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="1">
-        <v>0.6666666666666666</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14">
         <v>4</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -4852,29 +4852,29 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>4</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B18">
         <v>3</v>
@@ -4888,16 +4888,16 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19">
         <v>3</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="1">
-        <v>1</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -4916,21 +4916,21 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B21">
         <v>7</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1">
-        <v>0.5714285714285714</v>
+        <v>0.7142857142857143</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -4958,7 +4958,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B24">
         <v>5</v>
@@ -4986,7 +4986,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26">
         <v>5</v>
@@ -5000,7 +5000,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>7</v>
@@ -5014,16 +5014,16 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -5048,10 +5048,10 @@
         <v>4</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -5070,16 +5070,16 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="1">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -5098,16 +5098,16 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B34">
         <v>7</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" s="1">
-        <v>0.4285714285714285</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -5146,15 +5146,15 @@
         <v>4</v>
       </c>
       <c r="C37">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D37" s="1">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -5168,7 +5168,7 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -5224,7 +5224,7 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B43">
         <v>5</v>
@@ -5238,7 +5238,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B44">
         <v>2</v>
@@ -5252,7 +5252,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45">
         <v>2</v>
@@ -5266,7 +5266,7 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B46">
         <v>3</v>
@@ -5280,21 +5280,21 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47">
         <v>5</v>
       </c>
       <c r="C47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D47" s="1">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48">
         <v>5</v>

</xml_diff>